<commit_message>
Added support for publications
</commit_message>
<xml_diff>
--- a/src/data/publications.xlsx
+++ b/src/data/publications.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$M$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$2:$O$11</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
   <si>
     <t>SNo</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Forum</t>
   </si>
   <si>
-    <t>PublishDate</t>
-  </si>
-  <si>
     <t>Likes</t>
   </si>
   <si>
@@ -219,6 +216,42 @@
   </si>
   <si>
     <t>Data Science Central</t>
+  </si>
+  <si>
+    <t>Excerpt</t>
+  </si>
+  <si>
+    <t>In this post, we review the processes that development teams should follow during the SDLC in order to create high-quality, and highly-secure, software.</t>
+  </si>
+  <si>
+    <t>https://dz2cdn4.dzone.com/thumbnail?fid=7080427&amp;w=240</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>https://dz2cdn1.dzone.com/thumbnail?fid=8194084&amp;w=240</t>
+  </si>
+  <si>
+    <t>https://dz2cdn3.dzone.com/thumbnail?fid=6981778&amp;w=240</t>
+  </si>
+  <si>
+    <t>https://dz2cdn4.dzone.com/thumbnail?fid=7284279&amp;w=240</t>
+  </si>
+  <si>
+    <t>https://dz2cdn2.dzone.com/thumbnail?fid=3442945&amp;w=240</t>
+  </si>
+  <si>
+    <t>https://api.ning.com/files/I5Q3A4NUOoKZu3PsD7oI2m9IbFScacCiYpTSXrD-ic*FRdqF8dgLFro4rZl6kZhAw2fLcd3mPKrYAkQBg1IfwS3HdI*hCm9I/genericavatar.png?width=184&amp;height=184&amp;crop=1%3A1</t>
+  </si>
+  <si>
+    <t>https://kaggle2.blob.core.windows.net/avatars/images/104367-kg.JPG</t>
+  </si>
+  <si>
+    <t>https://3ovyg21t17l11k49tk1oma21-wpengine.netdna-ssl.com/wp-content/uploads/2018/01/Shashank-Shekhar-Singh_avatar_1516221294-96x96.jpg</t>
+  </si>
+  <si>
+    <t>PublishedOn</t>
   </si>
 </sst>
 </file>
@@ -228,7 +261,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-14009]yyyy/mm/dd;@"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +272,14 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,10 +302,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -274,11 +316,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -591,26 +638,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EA1E9B2-5A96-48ED-8728-69922F653AFB}">
-  <dimension ref="B2:M15"/>
+  <dimension ref="B2:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="4" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71" style="2" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" style="2"/>
-    <col min="5" max="5" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" style="2" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="2"/>
-    <col min="13" max="13" width="15.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="52.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="86.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="2"/>
+    <col min="6" max="6" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="2" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="2"/>
+    <col min="11" max="11" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="7" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="2"/>
+    <col min="15" max="15" width="15.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -620,384 +669,452 @@
       <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="L2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J3" s="5">
+      <c r="J3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="6">
         <v>43152</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="M3" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="I4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="5">
+      <c r="J4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="6">
         <v>43150</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="M4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" s="5">
+      <c r="J5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L5" s="6">
         <v>43101</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="M5" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="I6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="5">
+        <v>25</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="6">
         <v>43148</v>
       </c>
-      <c r="K6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="M6" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="5">
+      <c r="J7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="L7" s="6">
         <v>43143</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="M7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>6</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J8" s="5">
+      <c r="J8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="6">
         <v>43143</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="M8" s="2" t="s">
-        <v>11</v>
+        <v>42</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>7</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>23</v>
+      <c r="G9" s="5" t="s">
+        <v>71</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J9" s="5">
+        <v>22</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L9" s="6">
         <v>43130</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="M9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="5">
+      <c r="J10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L10" s="6">
         <v>43121</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="M10" s="2" t="s">
-        <v>11</v>
+        <v>41</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>9</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="5">
+      <c r="K11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L11" s="6">
         <v>43121</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="M11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="J15" s="5"/>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="L15" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1" xr:uid="{47D485D3-4E83-431A-A741-F88CB6C82886}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{0D11BA51-2549-4236-B11D-0B42A8406BF7}"/>
+    <hyperlink ref="G5" r:id="rId3" xr:uid="{C1B3A08A-EE59-4A47-86E0-A2E5D65384BA}"/>
+    <hyperlink ref="G8" r:id="rId4" xr:uid="{D1DC4E5F-E666-433F-936F-0BA9235B7246}"/>
+    <hyperlink ref="G10" r:id="rId5" xr:uid="{77171B93-B79C-44A2-AA74-6F6B9CF95CAA}"/>
+    <hyperlink ref="G11" r:id="rId6" xr:uid="{109A707D-7316-4247-AABB-A10120C074EE}"/>
+    <hyperlink ref="G9" r:id="rId7" xr:uid="{EB67B55F-3AC0-4699-8918-30B0B5F3C9C4}"/>
+    <hyperlink ref="G7" r:id="rId8" xr:uid="{4E3C8D77-D5D6-4947-AFD8-83027B64CD1C}"/>
+    <hyperlink ref="G6" r:id="rId9" xr:uid="{44A29E2E-DDC6-40AC-AAC4-9F09C6D578A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>